<commit_message>
Added systematic uncertainty to ball drop
</commit_message>
<xml_diff>
--- a/TerrenceKaiExperiment2.xlsx
+++ b/TerrenceKaiExperiment2.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t>Run #1</t>
   </si>
@@ -98,6 +98,15 @@
   <si>
     <t>g (m/s/s)</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Statistical Uncertainty</t>
+  </si>
+  <si>
+    <t>Systematic Uncertainty</t>
+  </si>
 </sst>
 </file>
 
@@ -152,8 +161,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,11 +174,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,20 +459,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W67"/>
+  <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -467,7 +480,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -499,7 +512,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -531,7 +544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -578,7 +591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9.4650999999999999E-2</v>
       </c>
@@ -586,6 +599,10 @@
         <f>(2/(A6 + B7)) * ((0.455/B7) - (0.08/A6))</f>
         <v>10.032046818127405</v>
       </c>
+      <c r="D6">
+        <f>(2/(A6+B7))*((0.4545/B7)-(0.0795/A6))</f>
+        <v>10.050869351109874</v>
+      </c>
       <c r="F6">
         <v>9.4669000000000003E-2</v>
       </c>
@@ -593,6 +610,10 @@
         <f>(2/(F6 + G7)) * ((0.54/G7) - (0.08/F6))</f>
         <v>10.056626785343727</v>
       </c>
+      <c r="I6">
+        <f>(2/(F6 + G7)) * ((0.5395/G7) - (0.0795/F6))</f>
+        <v>10.075757959045118</v>
+      </c>
       <c r="K6">
         <v>9.6704999999999999E-2</v>
       </c>
@@ -600,6 +621,10 @@
         <f>(2/(K6 + L7)) * ((0.63/L7) - (0.08/K6))</f>
         <v>10.048897385878302</v>
       </c>
+      <c r="N6">
+        <f>(2/(K6+L7))*((0.6295/L7)-(0.0795/K6))</f>
+        <v>10.067205490301527</v>
+      </c>
       <c r="P6">
         <v>9.7712999999999994E-2</v>
       </c>
@@ -607,6 +632,10 @@
         <f>(2/(P6+Q7))*((0.27/Q7)-(0.08/P6))</f>
         <v>10.332002536883326</v>
       </c>
+      <c r="S6">
+        <f>(2/(P6+Q7))*((0.2695/Q7)-(0.0795/P6))</f>
+        <v>10.343955134356923</v>
+      </c>
       <c r="U6">
         <v>0.100465</v>
       </c>
@@ -614,25 +643,49 @@
         <f>(2/(U6+V7))*((0.74/V7)-(0.08/U6))</f>
         <v>10.041135395106576</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X6">
+        <f>(2/(U6+V7))*((0.7395/V7)-(0.0795/U6))</f>
+        <v>10.05795455237498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>0.19708999999999999</v>
       </c>
+      <c r="D7">
+        <f>(2/(A6 + B7)) * ((0.4555/B7) - (0.0805/A6))</f>
+        <v>10.013224285144938</v>
+      </c>
       <c r="G7">
         <v>0.221692</v>
       </c>
+      <c r="I7">
+        <f>(2/(F6 + G7)) * ((0.5405/G7) - (0.0805/F6))</f>
+        <v>10.03749561164233</v>
+      </c>
       <c r="L7">
         <v>0.24676699999999999</v>
       </c>
+      <c r="N7">
+        <f>(2/(K6 + L7)) * ((0.6305/L7) - (0.0805/K6))</f>
+        <v>10.030589281455075</v>
+      </c>
       <c r="Q7">
         <v>0.13395899999999999</v>
       </c>
+      <c r="S7">
+        <f>(2/(P6 + Q7)) * ((0.2705/Q7) - (0.0805/P6))</f>
+        <v>10.320049939409726</v>
+      </c>
       <c r="V7">
         <v>0.27564699999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X7">
+        <f>(2/(U6 + V7)) * ((0.7405/V7) - (0.0805/U6))</f>
+        <v>10.024316237838175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9.5536999999999997E-2</v>
       </c>
@@ -669,7 +722,7 @@
         <v>10.06201907530107</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>0.197577</v>
       </c>
@@ -686,7 +739,7 @@
         <v>0.27523799999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9.8991999999999997E-2</v>
       </c>
@@ -723,7 +776,7 @@
         <v>10.042970406485617</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>0.197937</v>
       </c>
@@ -740,7 +793,7 @@
         <v>0.27452799999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9.4627000000000003E-2</v>
       </c>
@@ -777,7 +830,7 @@
         <v>10.027414978386554</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>0.197214</v>
       </c>
@@ -794,7 +847,7 @@
         <v>0.27573300000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>9.1489000000000001E-2</v>
       </c>
@@ -831,7 +884,7 @@
         <v>10.038041191613004</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>0.19619</v>
       </c>
@@ -848,7 +901,7 @@
         <v>0.27376499999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9.1579999999999995E-2</v>
       </c>
@@ -884,7 +937,7 @@
         <v>10.039992788601188</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>0.19644500000000001</v>
       </c>
@@ -901,7 +954,7 @@
         <v>0.27522200000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9.5168000000000003E-2</v>
       </c>
@@ -937,7 +990,7 @@
         <v>10.038383040480573</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>0.19747500000000001</v>
       </c>
@@ -954,7 +1007,7 @@
         <v>0.27431800000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9.9975999999999995E-2</v>
       </c>
@@ -990,7 +1043,7 @@
         <v>10.088570274651648</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>0.198356</v>
       </c>
@@ -1007,7 +1060,7 @@
         <v>0.27428000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9.6097000000000002E-2</v>
       </c>
@@ -1043,7 +1096,7 @@
         <v>10.058594804886557</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>0.197546</v>
       </c>
@@ -1060,7 +1113,7 @@
         <v>0.27431299999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9.5362000000000002E-2</v>
       </c>
@@ -1096,7 +1149,7 @@
         <v>10.067490760973623</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>0.19732</v>
       </c>
@@ -1113,645 +1166,756 @@
         <v>0.27302799999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(C6,C8,C10,C12,C14,C16,C18,C20,C22,C24)</f>
+        <v>10.029329970343353</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26">
+        <f>AVERAGE(H6,H8,H10,H12,H14,H16,H18,H20,H22,H24)</f>
+        <v>10.031211161002906</v>
+      </c>
+      <c r="M26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26">
+        <f>AVERAGE(M6,M8,M10,M12,M14,M16,M18,M20,M22,M24)</f>
+        <v>10.073616732687491</v>
+      </c>
+      <c r="R26" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26">
+        <f>AVERAGE(R6,R8,R10,R12,R14,R16,R18,R20,R22,R24)</f>
+        <v>10.325256330173302</v>
+      </c>
+      <c r="W26" t="s">
+        <v>22</v>
+      </c>
+      <c r="X26">
+        <f>AVERAGE(W6,W8,W10,W12,W14,W16,W18,W20,W22,W24)</f>
+        <v>10.05046127164864</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <f>_xlfn.STDEV.S(C6,C8,C10,C12,C14,C16,C18,C20,C22,C24,D26)/SQRT(10)</f>
+        <v>3.7447856647161845E-3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27">
+        <f>_xlfn.STDEV.S(H6,H8,H10,H12,H14,H16,H18,H20,H22,H24)/SQRT(10)</f>
+        <v>7.9277018181930833E-3</v>
+      </c>
+      <c r="M27" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27">
+        <f>_xlfn.STDEV.S(M6,M8,M10,M12,M14,M16,M18,M20,M22,M24)/SQRT(10)</f>
+        <v>6.6997627813884459E-3</v>
+      </c>
+      <c r="R27" t="s">
+        <v>23</v>
+      </c>
+      <c r="S27">
+        <f>_xlfn.STDEV.S(R6,R8,R10,R12,R14,R16,R18,R20,R22,R24)/SQRT(10)</f>
+        <v>2.9059441403360073E-3</v>
+      </c>
+      <c r="W27" t="s">
+        <v>23</v>
+      </c>
+      <c r="X27">
+        <f>_xlfn.STDEV.S(W6,W8,W10,W12,W14,W16,W18,W20,W22,W24)/SQRT(10)</f>
+        <v>5.7984525383928632E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <f>(D6-D7)/2</f>
+        <v>1.8822532982468054E-2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28">
+        <f>(I6 - I7)/2</f>
+        <v>1.9131173701394388E-2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28">
+        <f>(N6-N7)/2</f>
+        <v>1.8308104423225835E-2</v>
+      </c>
+      <c r="R28" t="s">
+        <v>24</v>
+      </c>
+      <c r="S28">
+        <f>(S6-S7)/2</f>
+        <v>1.1952597473598559E-2</v>
+      </c>
+      <c r="W28" t="s">
+        <v>24</v>
+      </c>
+      <c r="X28">
+        <f>(X6-X7)/2</f>
+        <v>1.6819157268402662E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>17</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E35" t="s">
         <v>17</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I35" t="s">
         <v>17</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>18</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E36" t="s">
         <v>18</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I36" t="s">
         <v>18</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M36" t="s">
         <v>18</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="Q36" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>0.68</v>
-      </c>
-      <c r="E33">
-        <v>0.51</v>
-      </c>
-      <c r="I33">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="M33">
-        <v>0.83</v>
-      </c>
-      <c r="Q33">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>0.69</v>
-      </c>
-      <c r="E34">
-        <v>0.52</v>
-      </c>
-      <c r="I34">
-        <v>1.17</v>
-      </c>
-      <c r="M34">
-        <v>0.84</v>
-      </c>
-      <c r="Q34">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>0.7</v>
-      </c>
-      <c r="E35">
-        <v>0.53</v>
-      </c>
-      <c r="I35">
-        <v>1.18</v>
-      </c>
-      <c r="M35">
-        <v>0.85</v>
-      </c>
-      <c r="Q35">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>0.71</v>
-      </c>
-      <c r="E36">
-        <v>0.54</v>
-      </c>
-      <c r="I36">
-        <v>1.19</v>
-      </c>
-      <c r="M36">
-        <v>0.86</v>
-      </c>
-      <c r="Q36">
-        <v>0.47</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
       <c r="E37">
-        <v>0.55000000000000004</v>
+        <v>0.51</v>
       </c>
       <c r="I37">
-        <v>1.2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="M37">
-        <v>0.86</v>
+        <v>0.83</v>
       </c>
       <c r="Q37">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>0.73</v>
+        <v>0.69</v>
       </c>
       <c r="E38">
-        <v>0.55000000000000004</v>
+        <v>0.52</v>
       </c>
       <c r="I38">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
       <c r="M38">
-        <v>0.87</v>
+        <v>0.84</v>
       </c>
       <c r="Q38">
-        <v>0.49</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>0.73</v>
+        <v>0.7</v>
       </c>
       <c r="E39">
-        <v>0.56000000000000005</v>
+        <v>0.53</v>
       </c>
       <c r="I39">
-        <v>1.21</v>
+        <v>1.18</v>
       </c>
       <c r="M39">
-        <v>0.88</v>
+        <v>0.85</v>
       </c>
       <c r="Q39">
-        <v>0.49</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="E40">
-        <v>0.56999999999999995</v>
+        <v>0.54</v>
       </c>
       <c r="I40">
-        <v>1.22</v>
+        <v>1.19</v>
       </c>
       <c r="M40">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="Q40">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>0.75</v>
+        <v>0.72</v>
       </c>
       <c r="E41">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I41">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="M41">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="Q41">
-        <v>0.51</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
       <c r="E42">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I42">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
       <c r="M42">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="Q42">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="E43">
-        <v>0.59</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="I43">
-        <v>1.24</v>
+        <v>1.21</v>
       </c>
       <c r="M43">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="Q43">
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="E44">
-        <v>0.59</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="I44">
-        <v>1.24</v>
+        <v>1.22</v>
       </c>
       <c r="M44">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="Q44">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="E45">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I45">
-        <v>1.25</v>
+        <v>1.22</v>
       </c>
       <c r="M45">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="Q45">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="E46">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I46">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="M46">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="Q46">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
       <c r="E47">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="I47">
-        <v>1.26</v>
+        <v>1.24</v>
       </c>
       <c r="M47">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="Q47">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
       <c r="E48">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="I48">
-        <v>1.26</v>
+        <v>1.24</v>
       </c>
       <c r="M48">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="Q48">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="E49">
-        <v>0.62</v>
+        <v>0.6</v>
       </c>
       <c r="I49">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="M49">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="Q49">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="E50">
-        <v>0.62</v>
+        <v>0.6</v>
       </c>
       <c r="I50">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="M50">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="Q50">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="E51">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="I51">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
       <c r="M51">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="Q51">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="E52">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="I52">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
       <c r="M52">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="Q52">
-        <v>0.56999999999999995</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>0.81</v>
+        <v>0.79</v>
       </c>
       <c r="E53">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="I53">
-        <v>1.29</v>
+        <v>1.27</v>
       </c>
       <c r="M53">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="Q53">
-        <v>0.56999999999999995</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>0.81</v>
+        <v>0.79</v>
       </c>
       <c r="E54">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="I54">
-        <v>1.29</v>
+        <v>1.27</v>
       </c>
       <c r="M54">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="Q54">
-        <v>0.56999999999999995</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>0.81</v>
+        <v>0.8</v>
       </c>
       <c r="E55">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="I55">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="M55">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="Q55">
-        <v>0.57999999999999996</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="E56">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="I56">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="M56">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="Q56">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="E57">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="I57">
-        <v>1.31</v>
+        <v>1.29</v>
       </c>
       <c r="M57">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="Q57">
-        <v>0.59</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>0.83</v>
+        <v>0.81</v>
       </c>
       <c r="E58">
-        <v>0.66</v>
+        <v>0.64</v>
       </c>
       <c r="I58">
-        <v>1.31</v>
+        <v>1.29</v>
       </c>
       <c r="M58">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="Q58">
-        <v>0.59</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>0.83</v>
+        <v>0.81</v>
       </c>
       <c r="E59">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="I59">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="M59">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="Q59">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="E60">
-        <v>0.67</v>
+        <v>0.65</v>
       </c>
       <c r="I60">
-        <v>1.32</v>
+        <v>1.3</v>
       </c>
       <c r="M60">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="Q60">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="E61">
-        <v>0.67</v>
+        <v>0.65</v>
       </c>
       <c r="I61">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="M61">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="Q61">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="E62">
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
       <c r="I62">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="M62">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="Q62">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="E63">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="I63">
-        <v>1.33</v>
+        <v>1.31</v>
       </c>
       <c r="M63">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="Q63">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
       <c r="E64">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="I64">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="M64">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="Q64">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="E65">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="I65">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
       <c r="M65">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="Q65">
-        <v>0.62</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="E66">
-        <v>0.69</v>
+        <v>0.67</v>
       </c>
       <c r="I66">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
       <c r="M66">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="Q66">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67">
+        <v>0.84</v>
+      </c>
+      <c r="E67">
+        <v>0.68</v>
+      </c>
+      <c r="I67">
+        <v>1.33</v>
+      </c>
+      <c r="M67">
+        <v>0.99</v>
+      </c>
+      <c r="Q67">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>0.85</v>
+      </c>
+      <c r="E68">
+        <v>0.68</v>
+      </c>
+      <c r="I68">
+        <v>1.33</v>
+      </c>
+      <c r="M68">
+        <v>1</v>
+      </c>
+      <c r="Q68">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>0.85</v>
+      </c>
+      <c r="E69">
+        <v>0.68</v>
+      </c>
+      <c r="I69">
+        <v>1.34</v>
+      </c>
+      <c r="M69">
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A70">
         <v>0.86</v>
       </c>
-      <c r="E67">
+      <c r="E70">
         <v>0.69</v>
       </c>
-      <c r="I67">
+      <c r="I70">
         <v>1.34</v>
       </c>
-      <c r="M67">
+      <c r="M70">
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>0.86</v>
+      </c>
+      <c r="E71">
+        <v>0.69</v>
+      </c>
+      <c r="I71">
+        <v>1.34</v>
+      </c>
+      <c r="M71">
         <v>1.01</v>
       </c>
-      <c r="Q67">
+      <c r="Q71">
         <v>0.62</v>
       </c>
     </row>

</xml_diff>